<commit_message>
new internal dashboard example
</commit_message>
<xml_diff>
--- a/Inputs/Consultants Database.xlsx
+++ b/Inputs/Consultants Database.xlsx
@@ -1092,7 +1092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:K53"/>
+  <dimension ref="A3:K52"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A36" sqref="A36:XFD36"/>
@@ -1586,9 +1586,7 @@
       </c>
       <c r="F23" s="64" t="n"/>
     </row>
-    <row r="24" s="79">
-      <c r="C24" t="inlineStr"/>
-    </row>
+    <row r="24" s="79"/>
     <row r="25" s="79">
       <c r="B25" s="20" t="inlineStr">
         <is>
@@ -1782,9 +1780,7 @@
       </c>
       <c r="F35" s="6" t="n"/>
     </row>
-    <row r="36" s="79">
-      <c r="C36" t="inlineStr"/>
-    </row>
+    <row r="36" s="79"/>
     <row r="37" s="79">
       <c r="A37" t="inlineStr">
         <is>
@@ -1886,9 +1882,7 @@
       </c>
       <c r="F40" s="31" t="n"/>
     </row>
-    <row r="41" s="79">
-      <c r="C41" t="inlineStr"/>
-    </row>
+    <row r="41" s="79"/>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
@@ -1971,9 +1965,7 @@
         </is>
       </c>
     </row>
-    <row r="45" s="79">
-      <c r="C45" t="inlineStr"/>
-    </row>
+    <row r="45" s="79"/>
     <row r="46" s="79"/>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3321,7 +3313,6 @@
           <t>Interested (as of Jan 2018)</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4" s="79">
       <c r="A4" t="n">
@@ -3363,7 +3354,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr"/>
       <c r="R4" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/almorton03/</t>
@@ -3410,7 +3400,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr"/>
       <c r="R5" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/alison-amoroso-5a7a08/</t>
@@ -3508,7 +3497,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr"/>
       <c r="R7" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ami-lynch-ph-d-1b00014/</t>
@@ -3555,7 +3543,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr"/>
       <c r="R8" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ana-garcia-9b43a760/</t>
@@ -3602,7 +3589,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr"/>
       <c r="R9" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/andrew-jones-29637753/</t>
@@ -3720,7 +3706,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr"/>
       <c r="R11" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/anita-case-6502932/</t>
@@ -3833,7 +3818,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr"/>
       <c r="R13" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/belindagaston/</t>
@@ -3875,7 +3859,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q14" t="inlineStr"/>
       <c r="R14" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/thurma-goldman-a7228922/</t>
@@ -3988,7 +3971,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr"/>
       <c r="R16" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/carriemurthy/</t>
@@ -4035,7 +4017,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18" s="79">
       <c r="A18" t="n">
@@ -4106,7 +4087,6 @@
           <t>Interested (as of Mar 2018)</t>
         </is>
       </c>
-      <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19" s="79">
       <c r="A19" t="n">
@@ -4175,7 +4155,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20" s="79">
       <c r="A20" t="n">
@@ -4239,7 +4218,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21" s="79">
       <c r="A21" t="n">
@@ -4281,7 +4259,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22" s="79">
       <c r="A22" t="n">
@@ -4343,7 +4320,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23" s="79">
       <c r="A23" t="n">
@@ -4400,7 +4376,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24" s="79">
       <c r="A24" t="n">
@@ -4437,7 +4412,6 @@
           <t>Mexico</t>
         </is>
       </c>
-      <c r="Q24" t="inlineStr"/>
       <c r="R24" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/deborah-bickel-2335558/</t>
@@ -4494,7 +4468,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q25" t="inlineStr"/>
       <c r="R25" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/debbie-isenberg-b7371982/</t>
@@ -4541,7 +4514,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q26" t="inlineStr"/>
       <c r="R26" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/deborah-carpenter-a8952b4/</t>
@@ -4573,7 +4545,6 @@
         </is>
       </c>
       <c r="K27" s="72" t="n"/>
-      <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28" s="79">
       <c r="A28" t="n">
@@ -4615,7 +4586,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q28" t="inlineStr"/>
       <c r="R28" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/donna-durant-atkinson-5678127/</t>
@@ -4699,7 +4669,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30" s="79">
       <c r="A30" t="n">
@@ -4736,7 +4705,6 @@
           <t>Cameroon</t>
         </is>
       </c>
-      <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31" s="79">
       <c r="A31" t="n">
@@ -4907,7 +4875,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q33" t="inlineStr"/>
       <c r="R33" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/elizabeth-c-b3968327/</t>
@@ -4954,7 +4921,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q34" t="inlineStr"/>
       <c r="R34" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/emily-abbruzzi-0a795164/</t>
@@ -5001,7 +4967,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q35" t="inlineStr"/>
       <c r="R35" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/drerikacopeland/</t>
@@ -5048,7 +5013,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q36" t="inlineStr"/>
       <c r="R36" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/erin-loomis-483a3920/</t>
@@ -5095,7 +5059,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q37" t="inlineStr"/>
       <c r="R37" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/eunice-mafundikwa-b3894b35/</t>
@@ -5142,7 +5105,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q38" t="inlineStr"/>
       <c r="R38" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/everlyne-nyagaya-24053011/</t>
@@ -5194,7 +5156,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q39" t="inlineStr"/>
       <c r="R39" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/galenellis95959/</t>
@@ -5236,7 +5197,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q40" t="inlineStr"/>
       <c r="R40" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/gebeyehu-teferi-801157130/</t>
@@ -5283,7 +5243,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42" s="79">
       <c r="A42" t="n">
@@ -5325,7 +5284,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q42" t="inlineStr"/>
       <c r="R42" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/drimani/</t>
@@ -5458,7 +5416,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45" s="79">
       <c r="A45" t="n">
@@ -5500,7 +5457,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q45" t="inlineStr"/>
       <c r="R45" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jeananne-cappetta-81712a16/</t>
@@ -5593,7 +5549,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q47" t="inlineStr"/>
       <c r="R47" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jenny-namur-karp-2a82b414/</t>
@@ -5640,7 +5595,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q48" t="inlineStr"/>
       <c r="R48" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jocelynfranke/</t>
@@ -5687,7 +5641,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q49" t="inlineStr"/>
       <c r="R49" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/john-easterday-ph-d-75127316/</t>
@@ -5771,7 +5724,6 @@
           <t>Interested (as of Dec 2017)</t>
         </is>
       </c>
-      <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51" s="79">
       <c r="A51" t="n">
@@ -5813,7 +5765,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q51" t="inlineStr"/>
       <c r="R51" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/julieyegen/</t>
@@ -5850,7 +5801,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q52" t="inlineStr"/>
       <c r="R52" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/june-crandall-25821817/</t>
@@ -5912,7 +5862,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q53" t="inlineStr"/>
       <c r="R53" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/karenkwokfnpmph/</t>
@@ -5949,7 +5898,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q54" t="inlineStr"/>
       <c r="R54" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kevin-frissell-8a976113/</t>
@@ -6001,7 +5949,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q55" t="inlineStr"/>
       <c r="R55" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kristin-harkness-21247515/</t>
@@ -6033,7 +5980,6 @@
         </is>
       </c>
       <c r="K56" s="72" t="n"/>
-      <c r="Q56" t="inlineStr"/>
     </row>
     <row r="57" s="79">
       <c r="A57" t="n">
@@ -6075,7 +6021,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q57" t="inlineStr"/>
       <c r="R57" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/malikah-waajid-phd-6084901b/</t>
@@ -6207,7 +6152,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60" s="79">
       <c r="A60" t="n">
@@ -6239,7 +6183,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q60" t="inlineStr"/>
       <c r="R60" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/marianaserrani/</t>
@@ -6286,7 +6229,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q61" t="inlineStr"/>
       <c r="R61" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/marneena-evans-4181117b/</t>
@@ -6333,7 +6275,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q62" t="inlineStr"/>
       <c r="R62" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/martineetiennemesubidrph/</t>
@@ -6380,7 +6321,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q63" t="inlineStr"/>
       <c r="R63" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/melanie-chansky-5263b782/</t>
@@ -6422,7 +6362,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q64" t="inlineStr"/>
       <c r="R64" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/renibello/</t>
@@ -6469,7 +6408,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q65" t="inlineStr"/>
       <c r="R65" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/moses-busiga-69687916/</t>
@@ -6567,7 +6505,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q67" t="inlineStr"/>
       <c r="R67" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ndidiamutah/</t>
@@ -6614,7 +6551,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q68" t="inlineStr"/>
       <c r="R68" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/nina-freed-b459233a/</t>
@@ -6661,7 +6597,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q69" t="inlineStr"/>
       <c r="R69" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/nlucciola/</t>
@@ -6708,7 +6643,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q70" t="inlineStr"/>
       <c r="R70" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/busolaafolabi/</t>
@@ -6760,7 +6694,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q71" t="inlineStr"/>
       <c r="R71" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/patricia-andersen-44b03215a/</t>
@@ -6802,7 +6735,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q72" t="inlineStr"/>
       <c r="R72" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/phil-melemed-43132b4/</t>
@@ -6849,7 +6781,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q73" t="inlineStr"/>
       <c r="R73" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/polly-ross-6b38a69b/</t>
@@ -7013,7 +6944,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77" s="79">
       <c r="A77" t="n">
@@ -7136,7 +7066,6 @@
           <t>Recommended by Dr. Iriso Robert</t>
         </is>
       </c>
-      <c r="Q78" t="inlineStr"/>
     </row>
     <row r="79" s="79">
       <c r="A79" t="n">
@@ -7260,7 +7189,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q81" t="inlineStr"/>
       <c r="R81" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sandralparedes/</t>
@@ -7419,7 +7347,6 @@
           <t>Interested (as of Dec 2017)</t>
         </is>
       </c>
-      <c r="Q84" t="inlineStr"/>
       <c r="R84" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sureyya-e-hornston-13b75a92/</t>
@@ -7461,7 +7388,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q85" t="inlineStr"/>
       <c r="R85" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/teresa-strickler-6437616/</t>
@@ -7578,7 +7504,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q87" t="inlineStr"/>
       <c r="R87" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/tadler2/</t>
@@ -7630,7 +7555,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q88" t="inlineStr"/>
     </row>
     <row r="89" s="79">
       <c r="A89" t="n">
@@ -7682,7 +7606,6 @@
           <t>MO</t>
         </is>
       </c>
-      <c r="Q89" t="inlineStr"/>
       <c r="R89" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/valeri-lane-7934b110/</t>
@@ -7734,7 +7657,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q90" t="inlineStr"/>
     </row>
     <row r="91" s="79">
       <c r="A91" t="n">
@@ -7791,7 +7713,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q91" t="inlineStr"/>
       <c r="R91" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/chris-b-agala-phd-79b73879/</t>
@@ -7860,7 +7781,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q92" t="inlineStr"/>
     </row>
     <row r="93" s="79">
       <c r="A93" t="n">
@@ -7907,7 +7827,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q93" t="inlineStr"/>
       <c r="R93" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/donald-j-alcendor-47416925/</t>
@@ -7969,7 +7888,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q94" t="inlineStr"/>
       <c r="R94" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kristine-allen-mph-ches-1a928717/</t>
@@ -8044,7 +7962,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q95" t="inlineStr"/>
     </row>
     <row r="96" s="79">
       <c r="A96" t="n">
@@ -8108,7 +8025,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q96" t="inlineStr"/>
     </row>
     <row r="97" s="79">
       <c r="A97" t="n">
@@ -8223,8 +8139,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr"/>
     </row>
     <row r="99" s="79">
       <c r="A99" t="n">
@@ -8332,7 +8246,6 @@
           <t>MD</t>
         </is>
       </c>
-      <c r="P100" t="inlineStr"/>
       <c r="Q100" t="inlineStr">
         <is>
           <t>aniational leaders; Assigned Tasked: OY1 Consultants Flyer (April 2018)</t>
@@ -8401,7 +8314,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P101" t="inlineStr"/>
       <c r="Q101" t="inlineStr">
         <is>
           <t>Other contact: (213)-509-9811</t>
@@ -8458,7 +8370,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q102" t="inlineStr"/>
     </row>
     <row r="103" s="79">
       <c r="A103" t="n">
@@ -8512,8 +8423,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P103" t="inlineStr"/>
-      <c r="Q103" t="inlineStr"/>
     </row>
     <row r="104" s="79">
       <c r="A104" t="n">
@@ -8577,7 +8486,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P104" t="inlineStr"/>
       <c r="Q104" t="inlineStr">
         <is>
           <t>Other contact: (615) 293-5241</t>
@@ -8646,8 +8554,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P105" t="inlineStr"/>
-      <c r="Q105" t="inlineStr"/>
     </row>
     <row r="106" s="79">
       <c r="A106" t="n">
@@ -8694,8 +8600,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P106" t="inlineStr"/>
-      <c r="Q106" t="inlineStr"/>
     </row>
     <row r="107" s="79">
       <c r="A107" t="n">
@@ -8820,8 +8724,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P108" t="inlineStr"/>
-      <c r="Q108" t="inlineStr"/>
     </row>
     <row r="109" s="79">
       <c r="A109" t="n">
@@ -8948,8 +8850,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P110" t="inlineStr"/>
-      <c r="Q110" t="inlineStr"/>
     </row>
     <row r="111" s="79">
       <c r="A111" t="n">
@@ -9009,7 +8909,6 @@
           <t>Interested (as of Jan 2018)</t>
         </is>
       </c>
-      <c r="Q111" t="inlineStr"/>
     </row>
     <row r="112" s="79">
       <c r="A112" t="n">
@@ -9071,7 +8970,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q112" t="inlineStr"/>
       <c r="R112" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sofiacamposvp/</t>
@@ -9140,7 +9038,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P113" t="inlineStr"/>
       <c r="Q113" t="inlineStr">
         <is>
           <t>Other contact: (718) 588-4151</t>
@@ -9207,7 +9104,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q114" t="inlineStr"/>
       <c r="R114" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/vernell-chapman-5887a514/</t>
@@ -9266,8 +9162,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P115" t="inlineStr"/>
-      <c r="Q115" t="inlineStr"/>
     </row>
     <row r="116" s="79">
       <c r="A116" t="n">
@@ -9314,7 +9208,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q116" t="inlineStr"/>
     </row>
     <row r="117" s="79">
       <c r="A117" t="n">
@@ -9378,7 +9271,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P117" t="inlineStr"/>
       <c r="Q117" t="inlineStr">
         <is>
           <t>Assigned Task: OY1 Consultants Flyer (April 2018)</t>
@@ -9445,8 +9337,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P118" t="inlineStr"/>
-      <c r="Q118" t="inlineStr"/>
     </row>
     <row r="119" s="79">
       <c r="A119" t="n">
@@ -9505,7 +9395,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q119" t="inlineStr"/>
     </row>
     <row r="120" s="79">
       <c r="A120" t="n">
@@ -9567,8 +9456,6 @@
           <t>South Africa</t>
         </is>
       </c>
-      <c r="P120" t="inlineStr"/>
-      <c r="Q120" t="inlineStr"/>
     </row>
     <row r="121" s="79">
       <c r="A121" t="n">
@@ -9632,8 +9519,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P121" t="inlineStr"/>
-      <c r="Q121" t="inlineStr"/>
     </row>
     <row r="122" s="79">
       <c r="A122" t="n">
@@ -9694,8 +9579,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P122" t="inlineStr"/>
-      <c r="Q122" t="inlineStr"/>
     </row>
     <row r="123" s="79">
       <c r="A123" t="n">
@@ -9756,8 +9639,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P123" t="inlineStr"/>
-      <c r="Q123" t="inlineStr"/>
     </row>
     <row r="124" s="79">
       <c r="A124" t="n">
@@ -9821,8 +9702,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P124" t="inlineStr"/>
-      <c r="Q124" t="inlineStr"/>
     </row>
     <row r="125" s="79">
       <c r="A125" t="n">
@@ -9869,8 +9748,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P125" t="inlineStr"/>
-      <c r="Q125" t="inlineStr"/>
       <c r="R125" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/habeeb-fasuyi-b5183723/</t>
@@ -9922,7 +9799,6 @@
           <t>MD</t>
         </is>
       </c>
-      <c r="P126" t="inlineStr"/>
       <c r="Q126" s="80" t="inlineStr">
         <is>
           <t>https://www.cpas4you.com/industries/government-contractors/</t>
@@ -9979,7 +9855,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q127" t="inlineStr"/>
       <c r="R127" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/tai-edward-few-3440137/</t>
@@ -10036,7 +9911,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P128" t="inlineStr"/>
       <c r="Q128" t="inlineStr">
         <is>
           <t>Other contact: (301) 502-1053</t>
@@ -10073,8 +9947,6 @@
           <t>UK</t>
         </is>
       </c>
-      <c r="P129" t="inlineStr"/>
-      <c r="Q129" t="inlineStr"/>
     </row>
     <row r="130" s="79">
       <c r="A130" t="n">
@@ -10121,8 +9993,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P130" t="inlineStr"/>
-      <c r="Q130" t="inlineStr"/>
     </row>
     <row r="131" s="79">
       <c r="A131" t="n">
@@ -10179,7 +10049,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q131" t="inlineStr"/>
       <c r="R131" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/tesfayi-gebreselassie-0b9795173/</t>
@@ -10248,7 +10117,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P132" t="inlineStr"/>
       <c r="Q132" t="inlineStr">
         <is>
           <t>Skype: nancy.gellerman</t>
@@ -10319,8 +10187,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P133" t="inlineStr"/>
-      <c r="Q133" t="inlineStr"/>
     </row>
     <row r="134" s="79">
       <c r="A134" t="n">
@@ -10372,8 +10238,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P134" t="inlineStr"/>
-      <c r="Q134" t="inlineStr"/>
     </row>
     <row r="135" s="79">
       <c r="A135" t="n">
@@ -10439,8 +10303,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P135" t="inlineStr"/>
-      <c r="Q135" t="inlineStr"/>
     </row>
     <row r="136" s="79">
       <c r="A136" t="n">
@@ -10509,8 +10371,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P136" t="inlineStr"/>
-      <c r="Q136" t="inlineStr"/>
     </row>
     <row r="137" s="79">
       <c r="A137" t="n">
@@ -10651,8 +10511,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P138" t="inlineStr"/>
-      <c r="Q138" t="inlineStr"/>
     </row>
     <row r="139" s="79">
       <c r="A139" t="n">
@@ -10709,7 +10567,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q139" t="inlineStr"/>
       <c r="R139" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/seghenhaile/</t>
@@ -10780,8 +10637,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P140" t="inlineStr"/>
-      <c r="Q140" t="inlineStr"/>
     </row>
     <row r="141" s="79">
       <c r="A141" t="n">
@@ -10823,8 +10678,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="P141" t="inlineStr"/>
-      <c r="Q141" t="inlineStr"/>
       <c r="R141" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/michelle-paul-heelan-ph-d-765a7/</t>
@@ -10947,7 +10800,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q143" t="inlineStr"/>
       <c r="R143" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/kawonda-holland/</t>
@@ -11021,8 +10873,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P144" t="inlineStr"/>
-      <c r="Q144" t="inlineStr"/>
     </row>
     <row r="145" s="79">
       <c r="A145" t="n">
@@ -11157,8 +11007,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P146" t="inlineStr"/>
-      <c r="Q146" t="inlineStr"/>
     </row>
     <row r="147" s="79">
       <c r="A147" t="n">
@@ -11227,7 +11075,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q147" t="inlineStr"/>
     </row>
     <row r="148" s="79">
       <c r="A148" t="n">
@@ -11276,8 +11123,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P148" t="inlineStr"/>
-      <c r="Q148" t="inlineStr"/>
     </row>
     <row r="149" s="79">
       <c r="A149" t="n">
@@ -11339,7 +11184,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q149" t="inlineStr"/>
     </row>
     <row r="150" s="79">
       <c r="A150" t="n">
@@ -11403,8 +11247,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
     </row>
     <row r="151" s="79">
       <c r="A151" t="n">
@@ -11502,7 +11344,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q152" t="inlineStr"/>
       <c r="R152" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/rachel-kagel-0b03b67/</t>
@@ -11569,7 +11410,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q153" t="inlineStr"/>
       <c r="R153" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/katie-kampa-27b9a933/</t>
@@ -11640,8 +11480,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P154" t="inlineStr"/>
-      <c r="Q154" t="inlineStr"/>
     </row>
     <row r="155" s="79">
       <c r="A155" t="n">
@@ -11705,7 +11543,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q155" t="inlineStr"/>
     </row>
     <row r="156" s="79">
       <c r="A156" t="n">
@@ -11754,8 +11591,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P156" t="inlineStr"/>
-      <c r="Q156" t="inlineStr"/>
     </row>
     <row r="157" s="79">
       <c r="A157" t="n">
@@ -11807,8 +11642,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P157" t="inlineStr"/>
-      <c r="Q157" t="inlineStr"/>
       <c r="R157" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/leahkedar/</t>
@@ -11879,8 +11712,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P158" t="inlineStr"/>
-      <c r="Q158" t="inlineStr"/>
     </row>
     <row r="159" s="79">
       <c r="A159" t="n">
@@ -11937,7 +11768,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q159" t="inlineStr"/>
       <c r="R159" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/krivelyova-anna/</t>
@@ -12004,7 +11834,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q160" t="inlineStr"/>
       <c r="R160" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/nora-kuiper-325a8926/</t>
@@ -12046,8 +11875,6 @@
           <t>South Africa</t>
         </is>
       </c>
-      <c r="P161" t="inlineStr"/>
-      <c r="Q161" t="inlineStr"/>
     </row>
     <row r="162" s="79">
       <c r="A162" t="n">
@@ -12101,8 +11928,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P162" t="inlineStr"/>
-      <c r="Q162" t="inlineStr"/>
     </row>
     <row r="163" s="79">
       <c r="A163" t="n">
@@ -12169,7 +11994,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q163" t="inlineStr"/>
       <c r="R163" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/shayannemartin/</t>
@@ -12221,8 +12045,6 @@
           <t>South Africa</t>
         </is>
       </c>
-      <c r="P164" t="inlineStr"/>
-      <c r="Q164" t="inlineStr"/>
       <c r="R164" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/lyn-solomon-middleton-41b3946/</t>
@@ -12279,7 +12101,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q165" t="inlineStr"/>
     </row>
     <row r="166" s="79">
       <c r="A166" t="n">
@@ -12316,8 +12137,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P166" t="inlineStr"/>
-      <c r="Q166" t="inlineStr"/>
       <c r="R166" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/denisemishiwiec/</t>
@@ -12384,8 +12203,6 @@
           <t>Cameroon</t>
         </is>
       </c>
-      <c r="P167" t="inlineStr"/>
-      <c r="Q167" t="inlineStr"/>
     </row>
     <row r="168" s="79">
       <c r="A168" t="n">
@@ -12651,8 +12468,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P171" t="inlineStr"/>
-      <c r="Q171" t="inlineStr"/>
     </row>
     <row r="172" s="79">
       <c r="A172" t="n">
@@ -12706,8 +12521,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P172" t="inlineStr"/>
-      <c r="Q172" t="inlineStr"/>
     </row>
     <row r="173" s="79">
       <c r="A173" t="n">
@@ -12769,7 +12582,6 @@
           <t>Interested (as of Feb 2018)</t>
         </is>
       </c>
-      <c r="Q173" t="inlineStr"/>
       <c r="R173" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/ninon-elsie-ekoto-zang-1ab54055/</t>
@@ -12904,8 +12716,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P175" t="inlineStr"/>
-      <c r="Q175" t="inlineStr"/>
     </row>
     <row r="176" s="79">
       <c r="A176" t="n">
@@ -12969,8 +12779,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P176" t="inlineStr"/>
-      <c r="Q176" t="inlineStr"/>
     </row>
     <row r="177" s="79">
       <c r="A177" t="n">
@@ -13078,8 +12886,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P178" t="inlineStr"/>
-      <c r="Q178" t="inlineStr"/>
       <c r="R178" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/dustynpalmer/</t>
@@ -13121,7 +12927,6 @@
           <t>Canada</t>
         </is>
       </c>
-      <c r="P179" t="inlineStr"/>
       <c r="Q179" t="inlineStr">
         <is>
           <t>Education</t>
@@ -13219,7 +13024,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q181" t="inlineStr"/>
     </row>
     <row r="182" s="79">
       <c r="A182" t="n">
@@ -13351,7 +13155,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q183" t="inlineStr"/>
       <c r="R183" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jaclyn-perlman-mph-aba26610/</t>
@@ -13420,7 +13223,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P184" t="inlineStr"/>
       <c r="Q184" t="inlineStr">
         <is>
           <t>Other contact: (443) 287-6179; Home address: 8004 Blair Mill Drive Apartment 202 Silver Spring, Maryland 20910 Mobile: +1-404-484-1118 Email: TPoteat123@gmail.com</t>
@@ -13487,7 +13289,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q185" t="inlineStr"/>
       <c r="R185" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/debra-prosnitz/</t>
@@ -13556,7 +13357,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q186" t="inlineStr"/>
     </row>
     <row r="187" s="79">
       <c r="A187" t="n">
@@ -13618,7 +13418,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q187" t="inlineStr"/>
       <c r="R187" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/sujata-ram-14b5a46/</t>
@@ -13685,7 +13484,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q188" t="inlineStr"/>
       <c r="R188" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/marissa-robinson-72b1a1145/</t>
@@ -13759,7 +13557,6 @@
           <t>Interested (as of Apr 2018)</t>
         </is>
       </c>
-      <c r="Q189" t="inlineStr"/>
     </row>
     <row r="190" s="79">
       <c r="A190" t="n">
@@ -13808,8 +13605,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P190" t="inlineStr"/>
-      <c r="Q190" t="inlineStr"/>
     </row>
     <row r="191" s="79">
       <c r="A191" t="n">
@@ -13873,8 +13668,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P191" t="inlineStr"/>
-      <c r="Q191" t="inlineStr"/>
     </row>
     <row r="192" s="79">
       <c r="A192" t="n">
@@ -13926,8 +13719,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P192" t="inlineStr"/>
-      <c r="Q192" t="inlineStr"/>
       <c r="R192" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/neginshakibisavalan/</t>
@@ -13991,8 +13782,6 @@
           <t>Zambia</t>
         </is>
       </c>
-      <c r="P193" t="inlineStr"/>
-      <c r="Q193" t="inlineStr"/>
     </row>
     <row r="194" s="79">
       <c r="A194" t="n">
@@ -14044,7 +13833,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P194" t="inlineStr"/>
       <c r="Q194" t="inlineStr">
         <is>
           <t>Other contact: (703) 728-6548</t>
@@ -14111,7 +13899,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q195" t="inlineStr"/>
       <c r="R195" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/bella-siangonya-mph-02230719/</t>
@@ -14175,8 +13962,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P196" t="inlineStr"/>
-      <c r="Q196" t="inlineStr"/>
     </row>
     <row r="197" s="79">
       <c r="A197" t="n">
@@ -14237,8 +14022,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P197" t="inlineStr"/>
-      <c r="Q197" t="inlineStr"/>
     </row>
     <row r="198" s="79">
       <c r="A198" t="n">
@@ -14285,8 +14068,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P198" t="inlineStr"/>
-      <c r="Q198" t="inlineStr"/>
       <c r="R198" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/freya-spielberg-056a025a/</t>
@@ -14343,8 +14124,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P199" t="inlineStr"/>
-      <c r="Q199" t="inlineStr"/>
       <c r="R199" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/melanie-steilen-4b653b1/</t>
@@ -14413,8 +14192,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P200" t="inlineStr"/>
-      <c r="Q200" t="inlineStr"/>
     </row>
     <row r="201" s="79">
       <c r="A201" t="n">
@@ -14473,8 +14250,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P201" t="inlineStr"/>
-      <c r="Q201" t="inlineStr"/>
     </row>
     <row r="202" s="79">
       <c r="A202" t="n">
@@ -14526,7 +14301,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q202" t="inlineStr"/>
       <c r="R202" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/meghan-swor-a2008a17/</t>
@@ -14593,7 +14367,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q203" t="inlineStr"/>
       <c r="R203" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/annatarrant/</t>
@@ -14665,7 +14438,6 @@
           <t>Interested (as of Dec 2017)</t>
         </is>
       </c>
-      <c r="Q204" t="inlineStr"/>
     </row>
     <row r="205" s="79">
       <c r="A205" t="n">
@@ -14792,7 +14564,6 @@
           <t>Interested (as of May 2018)</t>
         </is>
       </c>
-      <c r="Q206" t="inlineStr"/>
     </row>
     <row r="207" s="79">
       <c r="A207" t="n">
@@ -14861,7 +14632,6 @@
           <t>Interested (as of Dec 2017)</t>
         </is>
       </c>
-      <c r="Q207" t="inlineStr"/>
     </row>
     <row r="208" s="79">
       <c r="A208" t="n">
@@ -14928,7 +14698,6 @@
           <t>Interested</t>
         </is>
       </c>
-      <c r="Q208" t="inlineStr"/>
       <c r="R208" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/oliviavelez/</t>
@@ -14992,7 +14761,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P209" t="inlineStr"/>
       <c r="Q209" t="inlineStr">
         <is>
           <t>www.glassjacobson.com</t>
@@ -15134,8 +14902,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="P211" t="inlineStr"/>
-      <c r="Q211" t="inlineStr"/>
     </row>
     <row r="212" s="79">
       <c r="A212" t="n">
@@ -15197,7 +14963,6 @@
           <t>Interested (as of Mar 2018)</t>
         </is>
       </c>
-      <c r="Q212" t="inlineStr"/>
     </row>
     <row r="213" s="79">
       <c r="A213" t="n">
@@ -15244,7 +15009,6 @@
           <t>VA</t>
         </is>
       </c>
-      <c r="Q213" t="inlineStr"/>
     </row>
     <row r="214" s="79">
       <c r="A214" t="n">
@@ -15281,7 +15045,6 @@
           <t>FL</t>
         </is>
       </c>
-      <c r="Q214" t="inlineStr"/>
     </row>
     <row r="215" s="79">
       <c r="A215" t="n">
@@ -15328,7 +15091,6 @@
           <t>TX</t>
         </is>
       </c>
-      <c r="Q215" t="inlineStr"/>
     </row>
     <row r="216" s="79">
       <c r="A216" t="n">
@@ -15375,7 +15137,6 @@
           <t>NJ</t>
         </is>
       </c>
-      <c r="Q216" t="inlineStr"/>
     </row>
     <row r="217" s="79">
       <c r="A217" t="n">
@@ -15422,7 +15183,6 @@
           <t>CO</t>
         </is>
       </c>
-      <c r="Q217" t="inlineStr"/>
     </row>
     <row r="218" s="79">
       <c r="A218" t="n">
@@ -15469,7 +15229,6 @@
           <t>CO</t>
         </is>
       </c>
-      <c r="Q218" t="inlineStr"/>
     </row>
     <row r="219" s="79">
       <c r="A219" t="n">
@@ -15516,7 +15275,6 @@
           <t>NC</t>
         </is>
       </c>
-      <c r="Q219" t="inlineStr"/>
     </row>
     <row r="220" s="79">
       <c r="A220" t="n">
@@ -15553,7 +15311,6 @@
           <t>NC</t>
         </is>
       </c>
-      <c r="Q220" t="inlineStr"/>
     </row>
     <row r="221" s="79">
       <c r="A221" t="n">
@@ -15595,7 +15352,6 @@
           <t>FL</t>
         </is>
       </c>
-      <c r="Q221" t="inlineStr"/>
     </row>
     <row r="222" s="79">
       <c r="A222" t="n">
@@ -15642,7 +15398,6 @@
           <t>NE</t>
         </is>
       </c>
-      <c r="Q222" t="inlineStr"/>
     </row>
     <row r="223" s="79">
       <c r="A223" t="n">
@@ -15689,7 +15444,6 @@
           <t>AZ</t>
         </is>
       </c>
-      <c r="Q223" t="inlineStr"/>
     </row>
     <row r="224" s="79">
       <c r="A224" t="n">
@@ -15736,7 +15490,6 @@
           <t>FL</t>
         </is>
       </c>
-      <c r="Q224" t="inlineStr"/>
     </row>
     <row r="225" s="79">
       <c r="A225" t="n">
@@ -15783,7 +15536,6 @@
           <t>NC</t>
         </is>
       </c>
-      <c r="Q225" t="inlineStr"/>
       <c r="R225" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/jan-williams-b7393a135/</t>
@@ -15835,7 +15587,6 @@
           <t>UT</t>
         </is>
       </c>
-      <c r="Q226" t="inlineStr"/>
     </row>
     <row r="227" s="79">
       <c r="A227" t="n">
@@ -15933,7 +15684,6 @@
           <t>MD</t>
         </is>
       </c>
-      <c r="Q228" t="inlineStr"/>
     </row>
     <row r="229" s="79">
       <c r="A229" t="n">
@@ -15980,7 +15730,6 @@
           <t>GA</t>
         </is>
       </c>
-      <c r="Q229" t="inlineStr"/>
     </row>
     <row r="230" s="79">
       <c r="A230" t="n">
@@ -16027,7 +15776,6 @@
           <t>GA</t>
         </is>
       </c>
-      <c r="Q230" t="inlineStr"/>
     </row>
     <row r="231" s="79">
       <c r="A231" t="n">
@@ -16074,7 +15822,6 @@
           <t>GA</t>
         </is>
       </c>
-      <c r="Q231" t="inlineStr"/>
     </row>
     <row r="232" s="79">
       <c r="A232" t="n">
@@ -16121,7 +15868,6 @@
           <t>GA</t>
         </is>
       </c>
-      <c r="Q232" t="inlineStr"/>
     </row>
     <row r="233" s="79">
       <c r="A233" t="n">
@@ -16163,7 +15909,6 @@
           <t>Washington D.C.</t>
         </is>
       </c>
-      <c r="Q233" t="inlineStr"/>
     </row>
     <row r="234" s="79">
       <c r="A234" t="n">
@@ -16210,7 +15955,6 @@
           <t>MD</t>
         </is>
       </c>
-      <c r="Q234" t="inlineStr"/>
     </row>
     <row r="235" s="79">
       <c r="A235" t="n">
@@ -16257,7 +16001,6 @@
           <t>MD</t>
         </is>
       </c>
-      <c r="Q235" t="inlineStr"/>
     </row>
     <row r="236" s="79">
       <c r="A236" t="n">
@@ -16294,7 +16037,6 @@
           <t>Australia</t>
         </is>
       </c>
-      <c r="Q236" t="inlineStr"/>
       <c r="R236" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/peter-hague-30487823/</t>
@@ -16435,7 +16177,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q240" t="inlineStr"/>
       <c r="R240" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/tammy-camillo-06724389/</t>
@@ -16476,7 +16217,6 @@
           <t>Puerto Rico</t>
         </is>
       </c>
-      <c r="Q241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -16522,7 +16262,6 @@
           <t>FL</t>
         </is>
       </c>
-      <c r="Q242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -16574,7 +16313,6 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="Q243" t="inlineStr"/>
       <c r="R243" s="80" t="inlineStr">
         <is>
           <t>https://www.linkedin.com/in/scott-stanberry-29a01612/</t>
@@ -22763,7 +22501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B939"/>
+  <dimension ref="A1:B940"/>
   <sheetViews>
     <sheetView topLeftCell="A315" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B328" sqref="B328"/>
@@ -32043,7 +31781,7 @@
       </c>
       <c r="B927" t="inlineStr">
         <is>
-          <t>Budget and fiscal management</t>
+          <t>Report Writing</t>
         </is>
       </c>
     </row>
@@ -32053,7 +31791,7 @@
       </c>
       <c r="B928" t="inlineStr">
         <is>
-          <t>Behavioral Science</t>
+          <t>Budget and fiscal management</t>
         </is>
       </c>
     </row>
@@ -32063,7 +31801,7 @@
       </c>
       <c r="B929" t="inlineStr">
         <is>
-          <t>State Compliance Monitoring</t>
+          <t>Behavioral Science</t>
         </is>
       </c>
     </row>
@@ -32073,7 +31811,7 @@
       </c>
       <c r="B930" t="inlineStr">
         <is>
-          <t>Clinic Operations</t>
+          <t>State Compliance Monitoring</t>
         </is>
       </c>
     </row>
@@ -32083,7 +31821,7 @@
       </c>
       <c r="B931" t="inlineStr">
         <is>
-          <t>Financial analysis &amp; management</t>
+          <t>Clinic Operations</t>
         </is>
       </c>
     </row>
@@ -32093,7 +31831,7 @@
       </c>
       <c r="B932" t="inlineStr">
         <is>
-          <t>Fund development &amp; Sustainability</t>
+          <t>Financial analysis &amp; management</t>
         </is>
       </c>
     </row>
@@ -32103,7 +31841,7 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>Grants management</t>
+          <t>Fund development &amp; Sustainability</t>
         </is>
       </c>
     </row>
@@ -32113,7 +31851,7 @@
       </c>
       <c r="B934" t="inlineStr">
         <is>
-          <t>Quality improvement and management</t>
+          <t>Grants management</t>
         </is>
       </c>
     </row>
@@ -32123,7 +31861,7 @@
       </c>
       <c r="B935" t="inlineStr">
         <is>
-          <t>Strategic planning</t>
+          <t>Quality improvement and management</t>
         </is>
       </c>
     </row>
@@ -32133,7 +31871,7 @@
       </c>
       <c r="B936" t="inlineStr">
         <is>
-          <t>Nurse/Administration</t>
+          <t>Strategic planning</t>
         </is>
       </c>
     </row>
@@ -32143,7 +31881,7 @@
       </c>
       <c r="B937" t="inlineStr">
         <is>
-          <t>Data collection, analysis and reporting</t>
+          <t>Nurse/Administration</t>
         </is>
       </c>
     </row>
@@ -32153,7 +31891,7 @@
       </c>
       <c r="B938" t="inlineStr">
         <is>
-          <t>Program evaluation &amp; analysis</t>
+          <t>Data collection, analysis and reporting</t>
         </is>
       </c>
     </row>
@@ -32162,6 +31900,16 @@
         <v>244</v>
       </c>
       <c r="B939" t="inlineStr">
+        <is>
+          <t>Program evaluation &amp; analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="n">
+        <v>244</v>
+      </c>
+      <c r="B940" t="inlineStr">
         <is>
           <t>Time-constrainted Financial Analysis</t>
         </is>
@@ -39465,7 +39213,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="438" man="1" max="16383" min="0"/>
   </rowBreaks>
-  <colBreaks/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>

</xml_diff>